<commit_message>
NewCustomer and CustomerList POM added
</commit_message>
<xml_diff>
--- a/resources/Customer.xlsx
+++ b/resources/Customer.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF10B0D0-9AFA-499E-8B07-FCA8310043A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2085" yWindow="1680" windowWidth="12825" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,30 +17,99 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>user1@uat.com</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>UAT</t>
-  </si>
-  <si>
-    <t>Yes</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>customerState</t>
+  </si>
+  <si>
+    <t>customerDistrict</t>
+  </si>
+  <si>
+    <t>customerTaluk</t>
+  </si>
+  <si>
+    <t>customerPostal</t>
+  </si>
+  <si>
+    <t>customerVillage</t>
+  </si>
+  <si>
+    <t>customerShopType</t>
+  </si>
+  <si>
+    <t>customerShopName</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>customerLocalName</t>
+  </si>
+  <si>
+    <t>customerVillageLocalName</t>
+  </si>
+  <si>
+    <t>customerPhoneNumber</t>
+  </si>
+  <si>
+    <t>customerPhoneNumber2</t>
+  </si>
+  <si>
+    <t>customerAddress</t>
+  </si>
+  <si>
+    <t>customerLandMark</t>
+  </si>
+  <si>
+    <t>customerLeisure</t>
+  </si>
+  <si>
+    <t>customerBreakTime</t>
+  </si>
+  <si>
+    <t>customerHasCooler</t>
+  </si>
+  <si>
+    <t>customerCoolerType</t>
+  </si>
+  <si>
+    <t>customerQualification</t>
+  </si>
+  <si>
+    <t>customerGrade</t>
+  </si>
+  <si>
+    <t>customerAvgSale</t>
+  </si>
+  <si>
+    <t>customerIsSmartPhoneUser</t>
+  </si>
+  <si>
+    <t>KARNATAKA</t>
+  </si>
+  <si>
+    <t>MANDYA</t>
+  </si>
+  <si>
+    <t>Break Time</t>
+  </si>
+  <si>
+    <t>afternoon</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>Grade A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,6 +165,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -142,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,9 +248,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,55 +492,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>123456</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -445,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
added Customer Creation Flow in app
</commit_message>
<xml_diff>
--- a/resources/Customer.xlsx
+++ b/resources/Customer.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C83087-55EA-46F0-B3CF-65C83C7DA527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56E3992-7F5B-4089-B3F5-55F11AFC2F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7065" yWindow="1770" windowWidth="12825" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>customerState</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>SSLC</t>
+  </si>
+  <si>
+    <t>Belakavadi</t>
   </si>
 </sst>
 </file>
@@ -528,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>